<commit_message>
Fix excel censistas y modificacion environment a java 17
</commit_message>
<xml_diff>
--- a/src/listas_de_manzanas/coordenadas_manzanas.xlsx
+++ b/src/listas_de_manzanas/coordenadas_manzanas.xlsx
@@ -1,16 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25329"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9FC5314D-D94C-4D51-AC60-AD75823027CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mariano\eclipse-workspace\sistema-de-censo\src\listas_de_manzanas\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -27,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Nro manzana</t>
   </si>
@@ -41,21 +45,12 @@
     <t>-34.51909573235544, -58.71988115476912</t>
   </si>
   <si>
-    <t>2.1</t>
-  </si>
-  <si>
     <t>-34.52637948225431, -58.71009645709745</t>
   </si>
   <si>
-    <t>0.5</t>
-  </si>
-  <si>
     <t>-34.528005863683184, -58.731039143342066</t>
   </si>
   <si>
-    <t>0.3</t>
-  </si>
-  <si>
     <t>-34.54045016573941, -58.72511682633027</t>
   </si>
   <si>
@@ -77,9 +72,6 @@
     <t>-34.553275292650206, -58.719442876513725</t>
   </si>
   <si>
-    <t>3.7</t>
-  </si>
-  <si>
     <t>-34.56213183370967, -58.70717317543131</t>
   </si>
   <si>
@@ -89,32 +81,29 @@
     <t>-34.5586715072938, -58.691521521470904</t>
   </si>
   <si>
-    <t>5.7</t>
-  </si>
-  <si>
     <t>-34.559881, -58.690311</t>
   </si>
   <si>
     <t>-34.558972, -58.690062</t>
   </si>
   <si>
-    <t>8, 9</t>
-  </si>
-  <si>
     <t>-34.558429, -58.689490</t>
   </si>
   <si>
     <t>-34.557740, -58.690400</t>
   </si>
   <si>
-    <t>7, 11</t>
+    <t>8,9</t>
+  </si>
+  <si>
+    <t>7,11</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -160,14 +149,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -481,21 +472,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.7109375" customWidth="1"/>
     <col min="2" max="2" width="40.7109375" customWidth="1"/>
     <col min="3" max="3" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -506,147 +497,147 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="C2" s="4">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>4</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>5</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>6</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>8</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>10</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>12</v>
+      </c>
+      <c r="C8" s="4">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>13</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>15</v>
+      </c>
+      <c r="C10" s="4">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="3">
+      <c r="B11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="5">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+      <c r="B12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="3">
+      <c r="B13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="5">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" t="s">
-        <v>26</v>
+        <v>19</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>